<commit_message>
Fix nuts, version 2
</commit_message>
<xml_diff>
--- a/jems-ui/e2e/cypress/fixtures/programme/TB-747-partner-export-de-de.xlsx
+++ b/jems-ui/e2e/cypress/fixtures/programme/TB-747-partner-export-de-de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jems\ems\jems-ui\e2e\cypress\fixtures\programme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC02347-A907-443D-A716-48BB87B32E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95900CC-C6D0-41D0-B07E-79F1DCD3FB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54600" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partner data" sheetId="1" r:id="rId1"/>
@@ -1079,7 +1079,7 @@
   <dimension ref="A1:DG11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
MP2-3849 update export templates, minor fixes
</commit_message>
<xml_diff>
--- a/jems-ui/e2e/cypress/fixtures/programme/TB-747-partner-export-de-de.xlsx
+++ b/jems-ui/e2e/cypress/fixtures/programme/TB-747-partner-export-de-de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jilic\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jems\ems\jems-ui\e2e\cypress\fixtures\programme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF9F280-F7D5-431D-A5C4-85CFF8A1C50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5E6990-A09F-43B3-93D7-C02ABE5DE01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29025" yWindow="3390" windowWidth="50220" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partner data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t>+0987654321</t>
+  </si>
+  <si>
+    <t>API generated other identifier description DE</t>
   </si>
 </sst>
 </file>
@@ -1067,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="CI1" workbookViewId="0">
+      <selection activeCell="CL14" sqref="CL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,7 +1776,7 @@
         <v>126</v>
       </c>
       <c r="CK2" s="12" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="CL2" s="12" t="s">
         <v>127</v>
@@ -2100,7 +2103,7 @@
         <v>160</v>
       </c>
       <c r="CK3" s="12" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="CL3" s="12" t="s">
         <v>161</v>
@@ -2427,7 +2430,7 @@
         <v>126</v>
       </c>
       <c r="CK4" s="12" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="CL4" s="12" t="s">
         <v>127</v>
@@ -2754,7 +2757,7 @@
         <v>160</v>
       </c>
       <c r="CK5" s="12" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="CL5" s="12" t="s">
         <v>161</v>
@@ -3081,7 +3084,7 @@
         <v>126</v>
       </c>
       <c r="CK6" s="12" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="CL6" s="12" t="s">
         <v>127</v>
@@ -3408,7 +3411,7 @@
         <v>160</v>
       </c>
       <c r="CK7" s="12" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="CL7" s="12" t="s">
         <v>161</v>
@@ -3735,7 +3738,7 @@
         <v>126</v>
       </c>
       <c r="CK8" s="12" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="CL8" s="12" t="s">
         <v>127</v>
@@ -4062,7 +4065,7 @@
         <v>126</v>
       </c>
       <c r="CK9" s="12" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="CL9" s="12" t="s">
         <v>127</v>
@@ -4389,7 +4392,7 @@
         <v>126</v>
       </c>
       <c r="CK10" s="19" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="CL10" s="19" t="s">
         <v>127</v>

</xml_diff>